<commit_message>
Identifying a student by email instead of name Added most of the README.md
</commit_message>
<xml_diff>
--- a/Test av gruppeoppsett.xlsx
+++ b/Test av gruppeoppsett.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719B6C94-2376-4A37-9AE9-547E557A7AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B3536-BDA8-4051-8DEE-22D63A53002E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>Kveldstid</t>
   </si>
   <si>
-    <t>std6;std7</t>
-  </si>
-  <si>
     <t>sgfdhgh</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>student28</t>
+  </si>
+  <si>
+    <t>student6;student7</t>
   </si>
 </sst>
 </file>
@@ -437,11 +437,11 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Starttidspunkt" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fullføringstidspunkt" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="E-postadresse" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Navn" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{9FCDA347-E786-4CC0-A8BF-82A8DF2920E7}" name="Brukernavn" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Programmeringserfaring?" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Arbeidstid?" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ønskede samarbeidspartnere? Separer med komma(,) eller semikolon(;)" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Navn" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{9FCDA347-E786-4CC0-A8BF-82A8DF2920E7}" name="Brukernavn" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Programmeringserfaring?" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Arbeidstid?" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Ønskede samarbeidspartnere? Separer med komma(,) eller semikolon(;)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +776,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
@@ -802,7 +802,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>15</v>
@@ -814,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -860,7 +860,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -887,7 +887,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
@@ -914,7 +914,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>19</v>
@@ -926,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>20</v>
@@ -955,7 +955,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -972,7 +972,7 @@
         <v>38</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>21</v>
@@ -984,7 +984,7 @@
         <v>52</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1001,7 +1001,7 @@
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>22</v>
@@ -1028,7 +1028,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>23</v>
@@ -1055,7 +1055,7 @@
         <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>24</v>
@@ -1067,7 +1067,7 @@
         <v>52</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1084,7 +1084,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>25</v>
@@ -1111,7 +1111,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>26</v>
@@ -1123,7 +1123,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1140,7 +1140,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>27</v>
@@ -1152,7 +1152,7 @@
         <v>52</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1169,7 +1169,7 @@
         <v>45</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>28</v>
@@ -1181,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1198,7 +1198,7 @@
         <v>46</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>29</v>
@@ -1210,7 +1210,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1227,7 +1227,7 @@
         <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>30</v>
@@ -1239,7 +1239,7 @@
         <v>52</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>31</v>
@@ -1268,7 +1268,7 @@
         <v>9</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1285,7 +1285,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>32</v>
@@ -1297,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1314,7 +1314,7 @@
         <v>50</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>33</v>
@@ -1326,7 +1326,7 @@
         <v>52</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1343,7 +1343,7 @@
         <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>34</v>
@@ -1361,13 +1361,13 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>8</v>
@@ -1376,7 +1376,7 @@
         <v>9</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1384,13 +1384,13 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>10</v>
@@ -1399,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1407,13 +1407,13 @@
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>8</v>
@@ -1422,7 +1422,7 @@
         <v>52</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1430,13 +1430,13 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>10</v>
@@ -1445,7 +1445,7 @@
         <v>9</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1453,13 +1453,13 @@
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>10</v>
@@ -1468,7 +1468,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1476,13 +1476,13 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>10</v>
@@ -1491,7 +1491,7 @@
         <v>52</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1499,13 +1499,13 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>10</v>
@@ -1514,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1522,13 +1522,13 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>10</v>
@@ -1537,7 +1537,7 @@
         <v>9</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added option to get, update and partner with students based on username Added debug option
</commit_message>
<xml_diff>
--- a/Test av gruppeoppsett.xlsx
+++ b/Test av gruppeoppsett.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrem\WebstormProjects\idi-project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46B3536-BDA8-4051-8DEE-22D63A53002E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2EE1B2-C9B4-4C42-BC45-4EFB789F35A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>